<commit_message>
test Mon Apr 15 14:15:26 EDT 2019
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/JOURNAL_AG/CapStone1/PimaMarket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A0A62E6-5454-374F-A1C6-911427CBDFD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE15AF2-2B6E-DE44-85F1-DDE0A9A76AC9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16160" xr2:uid="{F4295600-9C80-A643-954C-9D650226C7C3}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t xml:space="preserve">sk;nlkdns </t>
   </si>
   <si>
-    <t xml:space="preserve">;ldfm </t>
+    <t>;ldfm g</t>
   </si>
 </sst>
 </file>

</xml_diff>